<commit_message>
TestRail reports are added.
</commit_message>
<xml_diff>
--- a/Manual Portfolio 1.xlsx
+++ b/Manual Portfolio 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emirbugrairmak/Desktop/QA ŞABLONLARI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emirbugrairmak/Desktop/ Manual QA Testing Portfolio Project (Risk-Based)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94895FDD-87E1-5B4B-B493-CB7A838CC5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBEF2C0-9656-9D42-9748-DEA27E0C1C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30020" windowHeight="17400" activeTab="8" xr2:uid="{F9A2DE0A-47D4-9343-9AB5-0B0D544D5F8A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30020" windowHeight="17400" activeTab="7" xr2:uid="{F9A2DE0A-47D4-9343-9AB5-0B0D544D5F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="İş Gereksinimi" sheetId="5" r:id="rId1"/>
@@ -2113,7 +2113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2190,10 +2190,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5457,7 +5454,7 @@
       <c r="B1" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>403</v>
       </c>
       <c r="D1" s="10" t="s">
@@ -5496,9 +5493,9 @@
       <c r="O1" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="T1" s="33"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="T1" s="32"/>
     </row>
     <row r="2" spans="1:20" ht="115" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -5546,7 +5543,7 @@
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
-      <c r="R2" s="32"/>
+      <c r="R2" s="7"/>
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
     </row>
@@ -5843,7 +5840,7 @@
       <c r="N8" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="34" t="s">
         <v>449</v>
       </c>
       <c r="P8" s="7"/>
@@ -6760,7 +6757,7 @@
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
-      <c r="R26" s="32"/>
+      <c r="R26" s="7"/>
       <c r="S26" s="7"/>
       <c r="T26" s="7"/>
     </row>
@@ -6883,7 +6880,7 @@
       <c r="F29" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="G29" s="36" t="s">
+      <c r="G29" s="35" t="s">
         <v>522</v>
       </c>
       <c r="H29" s="7" t="s">
@@ -8533,8 +8530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84DE64E-5B28-6849-8A2B-E898CDFD5FB8}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8601,7 +8598,7 @@
       <c r="O1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="P1" s="33"/>
+      <c r="P1" s="32"/>
     </row>
     <row r="2" spans="1:16" ht="161" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -8646,7 +8643,7 @@
       <c r="N2" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="38" t="s">
         <v>577</v>
       </c>
       <c r="P2" s="7"/>
@@ -8688,7 +8685,7 @@
       <c r="L3" s="7" t="s">
         <v>583</v>
       </c>
-      <c r="M3" s="35" t="s">
+      <c r="M3" s="34" t="s">
         <v>449</v>
       </c>
       <c r="N3" s="7" t="s">
@@ -8907,7 +8904,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="32"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -9490,7 +9487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4401ED-CA29-6D4C-BB4C-DBA61A986E82}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -9504,96 +9501,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="37" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>551</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>552</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>553</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="37" x14ac:dyDescent="0.45">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>555</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="37">
         <v>8</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="37">
         <v>6</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="37">
         <v>1</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="37">
         <v>1</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" ht="37" x14ac:dyDescent="0.45">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>556</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="37">
         <v>9</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="37">
         <v>4</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="37">
         <v>2</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="37">
         <v>3</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="37" x14ac:dyDescent="0.45">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="37">
         <v>31</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="37">
         <v>23</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="37">
         <v>4</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="37">
         <v>4</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>